<commit_message>
fix the formula error
</commit_message>
<xml_diff>
--- a/data/relay_table.xlsx
+++ b/data/relay_table.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongzhao/Documents/Claude_Code/中转站对比小网页/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C4C312-43D9-4544-9335-3AA65A3A2FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3422A6DE-75FD-D14B-BE11-6ED1C071112D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relay_table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>中转站名称</t>
   </si>
@@ -70,9 +83,6 @@
     <t>富可敌国</t>
   </si>
   <si>
-    <t>37.5</t>
-  </si>
-  <si>
     <t>1.5</t>
   </si>
   <si>
@@ -82,18 +92,12 @@
     <t>[Tiger（虎）](https://tiger.bookapi.cc/ref/C5E3)</t>
   </si>
   <si>
-    <t>13.65</t>
-  </si>
-  <si>
     <t>1.3</t>
   </si>
   <si>
     <t>0.7</t>
   </si>
   <si>
-    <t>0.546</t>
-  </si>
-  <si>
     <t>最低充值50</t>
   </si>
   <si>
@@ -118,9 +122,6 @@
     <t>[DuckCoding（鸭）](https://duckcoding.com/register?aff=pQIu)</t>
   </si>
   <si>
-    <t>32.5</t>
-  </si>
-  <si>
     <t>主站可签到，令有[公益站](https://free.duckcoding.com/register?aff=ZRcQ)，kiro反代</t>
   </si>
   <si>
@@ -130,30 +131,18 @@
     <t>[NekoCode](https://nekocode.ai?aff=TRPTNGM8)</t>
   </si>
   <si>
-    <t>12.46</t>
-  </si>
-  <si>
-    <t>0.4984</t>
-  </si>
-  <si>
     <t>订阅制&lt;br /&gt;本统计按Pro套餐计算（299¥/月，可使用600$）</t>
   </si>
   <si>
     <t>[HorseCoding（马）](https://www.horsecoding.cc)</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>0.8</t>
   </si>
   <si>
     <t>0.9</t>
   </si>
   <si>
-    <t>0.72</t>
-  </si>
-  <si>
     <t>~~刚开业，优惠价为0.7RMB1刀~~</t>
   </si>
   <si>
@@ -172,9 +161,6 @@
     <t>[YesCode](https://co.yes.vg/register?ref=TongZhao)</t>
   </si>
   <si>
-    <t>18.75</t>
-  </si>
-  <si>
     <t>0.75</t>
   </si>
   <si>
@@ -185,9 +171,6 @@
   </si>
   <si>
     <t>[FoxCode(狐狸)](https://foxcode.rjj.cc/auth/register?aff=6W5J31UI)</t>
-  </si>
-  <si>
-    <t>52.5</t>
   </si>
   <si>
     <t>0.35</t>
@@ -257,9 +240,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -565,7 +549,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -591,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -639,187 +623,202 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
+      <c r="C3">
+        <f>25*D3*E3</f>
+        <v>37.5</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f>C3/25</f>
+        <v>1.5</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <f>25*D4*E4</f>
+        <v>22.75</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4">
+        <f t="shared" ref="F4:F13" si="0">C4/25</f>
+        <v>0.91</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C13" si="1">25*D5*E5</f>
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -827,92 +826,99 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>18.75</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
-        <v>51</v>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
-        <v>55</v>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>18.375</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.73499999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>13.75</v>
+      <c r="C13" s="2">
+        <f t="shared" si="1"/>
+        <v>13.750000000000002</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>59</v>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update HorseCoding price and add FoxCode tiered plans
- HorseCoding: 18 → 22.5
- FoxCode: 112.5 → 150, add 35/135/468 tier plans

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/relay_table.xlsx
+++ b/data/relay_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongzhao/Documents/Claude_Code/中转站对比小网页/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaos/developments/price_comparison/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1478A090-A9DA-474B-87AD-4DF375C629E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5D3F81-D58A-BA4C-8DAA-5B43412E8A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="1380" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relay_table" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>中转站名称</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <f>C3/25</f>
+        <f>E3*D3</f>
         <v>1.5</v>
       </c>
       <c r="G3">
@@ -666,8 +666,8 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F13" si="0">C4/25</f>
-        <v>0.91</v>
+        <f>E4*D4</f>
+        <v>0.90999999999999992</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -687,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C13" si="1">25*D5*E5</f>
+        <f t="shared" ref="C5:C16" si="0">25*D5*E5</f>
         <v>25</v>
       </c>
       <c r="D5" t="s">
@@ -697,7 +697,7 @@
         <v>25</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>E5*D5</f>
         <v>1</v>
       </c>
       <c r="G5">
@@ -718,7 +718,7 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
       <c r="D6" t="s">
@@ -728,7 +728,7 @@
         <v>19</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f>E6*D6</f>
         <v>1.3</v>
       </c>
       <c r="G6">
@@ -749,7 +749,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="D7">
@@ -759,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>E7*D7</f>
         <v>0.5</v>
       </c>
       <c r="G7">
@@ -780,8 +780,7 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>22.5</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -790,8 +789,8 @@
         <v>35</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.72</v>
+        <f>E8*D8</f>
+        <v>0.72000000000000008</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -811,7 +810,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="D9" t="s">
@@ -821,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f>E9*D9</f>
         <v>1.5</v>
       </c>
       <c r="G9">
@@ -842,7 +841,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D10" t="s">
@@ -852,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>E10*D10</f>
         <v>1</v>
       </c>
       <c r="G10">
@@ -873,7 +872,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18.75</v>
       </c>
       <c r="D11" t="s">
@@ -883,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f>E11*D11</f>
         <v>0.75</v>
       </c>
       <c r="G11">
@@ -904,8 +903,7 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>112.5</v>
+        <v>150</v>
       </c>
       <c r="D12">
         <v>0.75</v>
@@ -914,7 +912,7 @@
         <v>6</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>E12*D12</f>
         <v>4.5</v>
       </c>
       <c r="G12">
@@ -929,32 +927,122 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+      <c r="D13">
+        <v>0.35</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F16" si="1">E13*D13</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="G13">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <v>0.27</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1.62</v>
+      </c>
+      <c r="G14">
+        <v>135</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+      <c r="D15">
+        <v>0.23</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1.3800000000000001</v>
+      </c>
+      <c r="G15">
+        <v>468</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>13.750000000000002</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
-        <v>13.750000000000002</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="G13">
+      <c r="G16">
         <v>220</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I16" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>